<commit_message>
Obtencion de objetos Clientes
</commit_message>
<xml_diff>
--- a/ConnectionApp/src/FormatoSalidaLista.xlsx
+++ b/ConnectionApp/src/FormatoSalidaLista.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SERVICIO AL CLIENTE\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ale Rodriguez\Desktop\trabajos\ConnectionApp\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F1D7DCF-43B1-47DC-9693-7A8A47260B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{27526CF5-CFDD-41D4-AC25-3C7AAF83C79B}"/>
+    <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="208">
   <si>
     <t>Apellido, Nombre</t>
   </si>
@@ -148,9 +147,6 @@
   </si>
   <si>
     <t>HUDSON, AUSTIN</t>
-  </si>
-  <si>
-    <t>HUDSON, USTIN</t>
   </si>
   <si>
     <t>MARRERO, VICTOR</t>
@@ -657,7 +653,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1003,15 +999,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3EF1631-7336-4C36-A1FE-CC9221F09D81}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
     <col min="11" max="11" width="20.85546875" customWidth="1"/>
     <col min="12" max="12" width="22" customWidth="1"/>
     <col min="14" max="14" width="22.42578125" customWidth="1"/>
@@ -1562,7 +1559,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16">
         <v>105</v>
@@ -1597,7 +1594,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17">
         <v>101</v>
@@ -1632,7 +1629,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18">
         <v>102</v>
@@ -1667,7 +1664,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19">
         <v>104</v>
@@ -1702,7 +1699,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20">
         <v>109</v>
@@ -1737,7 +1734,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21">
         <v>203</v>
@@ -1772,7 +1769,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22">
         <v>208</v>
@@ -1787,7 +1784,7 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K22" s="1">
         <v>44456</v>
@@ -1807,7 +1804,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23">
         <v>304</v>
@@ -1842,7 +1839,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24">
         <v>301</v>
@@ -1877,7 +1874,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25">
         <v>103</v>
@@ -1912,7 +1909,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26">
         <v>105</v>
@@ -1947,7 +1944,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27">
         <v>109</v>
@@ -1982,7 +1979,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28">
         <v>102</v>
@@ -2017,7 +2014,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29">
         <v>303</v>
@@ -2052,7 +2049,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30">
         <v>210</v>
@@ -2067,7 +2064,7 @@
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K30" s="1">
         <v>44457</v>
@@ -2087,7 +2084,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31">
         <v>103</v>
@@ -2122,7 +2119,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B32">
         <v>105</v>
@@ -2157,7 +2154,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33">
         <v>107</v>
@@ -2192,7 +2189,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34">
         <v>202</v>
@@ -2227,7 +2224,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B35">
         <v>205</v>
@@ -2297,7 +2294,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B37">
         <v>208</v>
@@ -2312,7 +2309,7 @@
         <v>1</v>
       </c>
       <c r="J37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K37" s="1">
         <v>44458</v>
@@ -2332,7 +2329,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B38">
         <v>107</v>
@@ -2367,7 +2364,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B39">
         <v>101</v>
@@ -2402,7 +2399,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B40">
         <v>204</v>
@@ -2437,7 +2434,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B41">
         <v>105</v>
@@ -2472,7 +2469,7 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B42">
         <v>108</v>
@@ -2507,7 +2504,7 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B43">
         <v>104</v>
@@ -2542,7 +2539,7 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B44">
         <v>103</v>
@@ -2577,7 +2574,7 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B45">
         <v>206</v>
@@ -2612,7 +2609,7 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B46">
         <v>102</v>
@@ -2647,7 +2644,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B47">
         <v>208</v>
@@ -2662,7 +2659,7 @@
         <v>1</v>
       </c>
       <c r="J47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K47" s="1">
         <v>44459</v>
@@ -2682,7 +2679,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B48">
         <v>207</v>
@@ -2717,7 +2714,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B49">
         <v>105</v>
@@ -2752,7 +2749,7 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B50">
         <v>109</v>
@@ -2787,7 +2784,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B51">
         <v>205</v>
@@ -2822,7 +2819,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B52">
         <v>207</v>
@@ -2849,7 +2846,7 @@
         <v>1</v>
       </c>
       <c r="N52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O52">
         <v>0</v>
@@ -2860,7 +2857,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B53">
         <v>204</v>
@@ -2895,7 +2892,7 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B54">
         <v>106</v>
@@ -2930,7 +2927,7 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B55">
         <v>103</v>
@@ -2965,7 +2962,7 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B56">
         <v>101</v>
@@ -3000,7 +2997,7 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B57">
         <v>210</v>
@@ -3035,7 +3032,7 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B58">
         <v>107</v>
@@ -3070,7 +3067,7 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B59">
         <v>108</v>
@@ -3105,7 +3102,7 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B60">
         <v>303</v>
@@ -3140,7 +3137,7 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B61">
         <v>202</v>
@@ -3175,7 +3172,7 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B62">
         <v>207</v>
@@ -3210,7 +3207,7 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B63">
         <v>204</v>
@@ -3245,7 +3242,7 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B64">
         <v>208</v>
@@ -3260,7 +3257,7 @@
         <v>1</v>
       </c>
       <c r="J64" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K64" s="1">
         <v>44462</v>
@@ -3280,7 +3277,7 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B65">
         <v>206</v>
@@ -3315,7 +3312,7 @@
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B66">
         <v>108</v>
@@ -3350,7 +3347,7 @@
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B67">
         <v>103</v>
@@ -3385,7 +3382,7 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B68">
         <v>105</v>
@@ -3420,7 +3417,7 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B69">
         <v>106</v>
@@ -3455,7 +3452,7 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B70">
         <v>107</v>
@@ -3490,7 +3487,7 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B71">
         <v>104</v>
@@ -3525,7 +3522,7 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B72">
         <v>209</v>
@@ -3540,7 +3537,7 @@
         <v>1</v>
       </c>
       <c r="J72" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K72" s="1">
         <v>44462</v>
@@ -3560,7 +3557,7 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B73">
         <v>101</v>
@@ -3595,7 +3592,7 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B74">
         <v>210</v>
@@ -3610,7 +3607,7 @@
         <v>1</v>
       </c>
       <c r="J74" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K74" s="1">
         <v>44462</v>
@@ -3630,7 +3627,7 @@
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B75">
         <v>207</v>
@@ -3665,7 +3662,7 @@
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B76">
         <v>203</v>
@@ -3700,7 +3697,7 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B77">
         <v>202</v>
@@ -3735,7 +3732,7 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B78">
         <v>207</v>
@@ -3770,7 +3767,7 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B79">
         <v>102</v>
@@ -3805,7 +3802,7 @@
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B80">
         <v>203</v>
@@ -3840,7 +3837,7 @@
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B81">
         <v>303</v>
@@ -3875,7 +3872,7 @@
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B82">
         <v>210</v>
@@ -3890,7 +3887,7 @@
         <v>1</v>
       </c>
       <c r="J82" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K82" s="1">
         <v>44463</v>
@@ -3910,7 +3907,7 @@
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B83">
         <v>302</v>
@@ -3945,7 +3942,7 @@
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B84">
         <v>101</v>
@@ -3980,7 +3977,7 @@
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B85">
         <v>306</v>
@@ -4015,7 +4012,7 @@
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B86">
         <v>307</v>
@@ -4050,7 +4047,7 @@
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B87">
         <v>210</v>
@@ -4065,7 +4062,7 @@
         <v>1</v>
       </c>
       <c r="J87" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K87" s="1">
         <v>44464</v>
@@ -4085,7 +4082,7 @@
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B88">
         <v>202</v>
@@ -4120,7 +4117,7 @@
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B89">
         <v>303</v>
@@ -4155,7 +4152,7 @@
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B90">
         <v>209</v>
@@ -4170,7 +4167,7 @@
         <v>1</v>
       </c>
       <c r="J90" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K90" s="1">
         <v>44464</v>
@@ -4190,7 +4187,7 @@
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B91">
         <v>302</v>
@@ -4225,7 +4222,7 @@
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B92">
         <v>305</v>
@@ -4260,7 +4257,7 @@
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B93">
         <v>201</v>
@@ -4295,7 +4292,7 @@
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B94">
         <v>305</v>
@@ -4330,7 +4327,7 @@
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B95">
         <v>105</v>
@@ -4365,7 +4362,7 @@
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B96">
         <v>101</v>
@@ -4400,7 +4397,7 @@
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B97">
         <v>102</v>
@@ -4435,7 +4432,7 @@
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B98">
         <v>103</v>
@@ -4470,13 +4467,13 @@
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B99">
         <v>207</v>
       </c>
       <c r="C99" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H99">
         <v>2</v>
@@ -4497,7 +4494,7 @@
         <v>4</v>
       </c>
       <c r="N99" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O99">
         <v>0</v>
@@ -4508,7 +4505,7 @@
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B100">
         <v>302</v>
@@ -4543,7 +4540,7 @@
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B101">
         <v>107</v>
@@ -4578,7 +4575,7 @@
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B102">
         <v>107</v>
@@ -4613,7 +4610,7 @@
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B103">
         <v>204</v>
@@ -4648,7 +4645,7 @@
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B104">
         <v>303</v>
@@ -4683,7 +4680,7 @@
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B105">
         <v>102</v>
@@ -4718,7 +4715,7 @@
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B106">
         <v>306</v>
@@ -4753,7 +4750,7 @@
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B107">
         <v>108</v>
@@ -4788,7 +4785,7 @@
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B108">
         <v>103</v>
@@ -4823,7 +4820,7 @@
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B109">
         <v>201</v>
@@ -4858,7 +4855,7 @@
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B110">
         <v>105</v>
@@ -4893,7 +4890,7 @@
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B111">
         <v>109</v>
@@ -4928,7 +4925,7 @@
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B112">
         <v>105</v>
@@ -4963,7 +4960,7 @@
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B113">
         <v>103</v>
@@ -4998,7 +4995,7 @@
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B114">
         <v>106</v>
@@ -5033,7 +5030,7 @@
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B115">
         <v>302</v>
@@ -5068,7 +5065,7 @@
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B116">
         <v>206</v>
@@ -5103,7 +5100,7 @@
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B117">
         <v>107</v>
@@ -5138,7 +5135,7 @@
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B118">
         <v>208</v>
@@ -5153,7 +5150,7 @@
         <v>1</v>
       </c>
       <c r="J118" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K118" s="1">
         <v>44469</v>
@@ -5173,7 +5170,7 @@
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B119">
         <v>306</v>
@@ -5208,7 +5205,7 @@
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B120">
         <v>109</v>
@@ -5243,7 +5240,7 @@
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B121">
         <v>102</v>
@@ -5278,7 +5275,7 @@
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B122">
         <v>107</v>
@@ -5313,7 +5310,7 @@
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B123">
         <v>108</v>
@@ -5348,7 +5345,7 @@
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B124">
         <v>203</v>
@@ -5383,7 +5380,7 @@
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B125">
         <v>109</v>
@@ -5418,7 +5415,7 @@
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B126">
         <v>101</v>
@@ -5453,7 +5450,7 @@
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B127">
         <v>202</v>
@@ -5488,7 +5485,7 @@
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B128">
         <v>102</v>
@@ -5523,13 +5520,13 @@
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B129">
         <v>307</v>
       </c>
       <c r="C129" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H129">
         <v>4</v>
@@ -5550,7 +5547,7 @@
         <v>1</v>
       </c>
       <c r="N129" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O129">
         <v>0</v>
@@ -5561,7 +5558,7 @@
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B130">
         <v>302</v>
@@ -5596,7 +5593,7 @@
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B131">
         <v>102</v>
@@ -5631,7 +5628,7 @@
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B132">
         <v>103</v>
@@ -5666,7 +5663,7 @@
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B133">
         <v>106</v>
@@ -5701,7 +5698,7 @@
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B134">
         <v>105</v>
@@ -5736,7 +5733,7 @@
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B135">
         <v>104</v>
@@ -5771,7 +5768,7 @@
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B136">
         <v>107</v>
@@ -5806,7 +5803,7 @@
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B137">
         <v>201</v>
@@ -5841,7 +5838,7 @@
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B138">
         <v>107</v>
@@ -5876,7 +5873,7 @@
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B139">
         <v>103</v>
@@ -5911,7 +5908,7 @@
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B140">
         <v>107</v>
@@ -5946,7 +5943,7 @@
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B141">
         <v>103</v>
@@ -5981,7 +5978,7 @@
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B142">
         <v>109</v>
@@ -6016,7 +6013,7 @@
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B143">
         <v>102</v>
@@ -6051,7 +6048,7 @@
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B144">
         <v>105</v>
@@ -6086,7 +6083,7 @@
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B145">
         <v>301</v>
@@ -6121,7 +6118,7 @@
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B146">
         <v>107</v>
@@ -6156,7 +6153,7 @@
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B147">
         <v>208</v>
@@ -6171,7 +6168,7 @@
         <v>1</v>
       </c>
       <c r="J147" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K147" s="1">
         <v>44474</v>
@@ -6191,7 +6188,7 @@
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B148">
         <v>304</v>
@@ -6226,7 +6223,7 @@
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B149">
         <v>208</v>
@@ -6241,7 +6238,7 @@
         <v>1</v>
       </c>
       <c r="J149" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K149" s="1">
         <v>44474</v>
@@ -6261,7 +6258,7 @@
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B150">
         <v>108</v>
@@ -6296,7 +6293,7 @@
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B151">
         <v>108</v>
@@ -6331,7 +6328,7 @@
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B152">
         <v>103</v>
@@ -6366,7 +6363,7 @@
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B153">
         <v>201</v>
@@ -6401,7 +6398,7 @@
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B154">
         <v>209</v>
@@ -6416,7 +6413,7 @@
         <v>1</v>
       </c>
       <c r="J154" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K154" s="1">
         <v>44475</v>
@@ -6436,7 +6433,7 @@
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B155">
         <v>203</v>
@@ -6471,7 +6468,7 @@
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B156">
         <v>101</v>
@@ -6506,7 +6503,7 @@
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B157">
         <v>303</v>
@@ -6541,7 +6538,7 @@
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B158">
         <v>304</v>
@@ -6576,7 +6573,7 @@
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B159">
         <v>109</v>
@@ -6611,7 +6608,7 @@
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B160">
         <v>107</v>
@@ -6646,7 +6643,7 @@
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B161">
         <v>105</v>
@@ -6681,7 +6678,7 @@
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B162">
         <v>307</v>
@@ -6716,7 +6713,7 @@
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B163">
         <v>207</v>
@@ -6751,7 +6748,7 @@
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B164">
         <v>105</v>
@@ -6786,7 +6783,7 @@
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B165">
         <v>103</v>
@@ -6821,7 +6818,7 @@
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B166">
         <v>204</v>
@@ -6856,7 +6853,7 @@
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B167">
         <v>102</v>
@@ -6891,7 +6888,7 @@
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B168">
         <v>202</v>
@@ -6926,7 +6923,7 @@
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B169">
         <v>102</v>
@@ -6961,7 +6958,7 @@
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B170">
         <v>109</v>
@@ -6996,7 +6993,7 @@
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B171">
         <v>203</v>
@@ -7031,7 +7028,7 @@
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B172">
         <v>209</v>
@@ -7046,7 +7043,7 @@
         <v>1</v>
       </c>
       <c r="J172" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K172" s="1">
         <v>44477</v>
@@ -7066,7 +7063,7 @@
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B173">
         <v>104</v>
@@ -7101,7 +7098,7 @@
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B174">
         <v>106</v>
@@ -7136,7 +7133,7 @@
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B175">
         <v>302</v>
@@ -7171,7 +7168,7 @@
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B176">
         <v>107</v>
@@ -7206,7 +7203,7 @@
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B177">
         <v>108</v>
@@ -7241,7 +7238,7 @@
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B178">
         <v>208</v>
@@ -7256,7 +7253,7 @@
         <v>1</v>
       </c>
       <c r="J178" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K178" s="1">
         <v>44477</v>
@@ -7276,7 +7273,7 @@
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B179">
         <v>205</v>
@@ -7311,7 +7308,7 @@
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B180">
         <v>307</v>
@@ -7346,7 +7343,7 @@
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B181">
         <v>304</v>
@@ -7381,7 +7378,7 @@
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B182">
         <v>204</v>
@@ -7416,13 +7413,13 @@
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B183">
         <v>201</v>
       </c>
       <c r="C183" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H183">
         <v>2</v>
@@ -7443,7 +7440,7 @@
         <v>1</v>
       </c>
       <c r="N183" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O183">
         <v>0</v>
@@ -7454,7 +7451,7 @@
     </row>
     <row r="184" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B184">
         <v>301</v>
@@ -7489,7 +7486,7 @@
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B185">
         <v>101</v>
@@ -7524,7 +7521,7 @@
     </row>
     <row r="186" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B186">
         <v>106</v>
@@ -7559,7 +7556,7 @@
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B187">
         <v>107</v>
@@ -7594,7 +7591,7 @@
     </row>
     <row r="188" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B188">
         <v>108</v>
@@ -7629,7 +7626,7 @@
     </row>
     <row r="189" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B189">
         <v>105</v>
@@ -7664,7 +7661,7 @@
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B190">
         <v>109</v>
@@ -7699,7 +7696,7 @@
     </row>
     <row r="191" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B191">
         <v>306</v>
@@ -7734,7 +7731,7 @@
     </row>
     <row r="192" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B192">
         <v>307</v>
@@ -7769,7 +7766,7 @@
     </row>
     <row r="193" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B193">
         <v>303</v>
@@ -7804,7 +7801,7 @@
     </row>
     <row r="194" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B194">
         <v>101</v>
@@ -7839,57 +7836,57 @@
     </row>
     <row r="195" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
+        <v>204</v>
+      </c>
+      <c r="B195" t="s">
+        <v>204</v>
+      </c>
+      <c r="C195" t="s">
         <v>205</v>
       </c>
-      <c r="B195" t="s">
-        <v>205</v>
-      </c>
-      <c r="C195" t="s">
+      <c r="D195" t="s">
+        <v>204</v>
+      </c>
+      <c r="E195" t="s">
+        <v>204</v>
+      </c>
+      <c r="F195" t="s">
+        <v>204</v>
+      </c>
+      <c r="G195" t="s">
+        <v>204</v>
+      </c>
+      <c r="H195" t="s">
         <v>206</v>
       </c>
-      <c r="D195" t="s">
-        <v>205</v>
-      </c>
-      <c r="E195" t="s">
-        <v>205</v>
-      </c>
-      <c r="F195" t="s">
-        <v>205</v>
-      </c>
-      <c r="G195" t="s">
-        <v>205</v>
-      </c>
-      <c r="H195" t="s">
-        <v>207</v>
-      </c>
       <c r="I195" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J195" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K195" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L195" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M195" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="N195" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O195" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="P195" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="196" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C196">
         <v>193</v>

</xml_diff>